<commit_message>
update date 8-5-2025 revised awaiting concurence
</commit_message>
<xml_diff>
--- a/data/Bills-RUBIO-Present.xlsx
+++ b/data/Bills-RUBIO-Present.xlsx
@@ -414,9 +414,6 @@
     <t>Physicians and surgeons: special faculty permits: academic medical centers.</t>
   </si>
   <si>
-    <t>Senate - Unfinished Business</t>
-  </si>
-  <si>
     <t>SB-388</t>
   </si>
   <si>
@@ -625,6 +622,9 @@
   </si>
   <si>
     <t>Senate - B. P. &amp; E.D.</t>
+  </si>
+  <si>
+    <t>Senate - Waiting Concurence</t>
   </si>
 </sst>
 </file>
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1194,7 +1194,7 @@
         <v>15</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1794,12 +1794,12 @@
         <v>15</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>131</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>97</v>
@@ -1808,7 +1808,7 @@
         <v>8</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>10</v>
@@ -1819,7 +1819,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>124</v>
@@ -1828,18 +1828,18 @@
         <v>8</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>131</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>61</v>
@@ -1848,27 +1848,27 @@
         <v>8</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>15</v>
@@ -1879,7 +1879,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>61</v>
@@ -1888,27 +1888,27 @@
         <v>8</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>15</v>
@@ -1919,16 +1919,16 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>10</v>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>61</v>
@@ -1948,18 +1948,18 @@
         <v>8</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>116</v>
@@ -1968,7 +1968,7 @@
         <v>8</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>15</v>
@@ -1979,16 +1979,16 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>10</v>
@@ -1999,7 +1999,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>61</v>
@@ -2008,18 +2008,18 @@
         <v>8</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>61</v>
@@ -2028,7 +2028,7 @@
         <v>8</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>15</v>
@@ -2039,7 +2039,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>97</v>
@@ -2048,7 +2048,7 @@
         <v>8</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>15</v>
@@ -2059,16 +2059,16 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="C55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>10</v>
@@ -2079,7 +2079,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>61</v>
@@ -2088,18 +2088,18 @@
         <v>8</v>
       </c>
       <c r="D56" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>61</v>
@@ -2108,7 +2108,7 @@
         <v>8</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>10</v>
@@ -2119,16 +2119,16 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>10</v>
@@ -2139,7 +2139,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>61</v>
@@ -2148,7 +2148,7 @@
         <v>8</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>10</v>
@@ -2159,7 +2159,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>61</v>
@@ -2168,27 +2168,27 @@
         <v>8</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>15</v>
@@ -2199,7 +2199,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>61</v>
@@ -2208,7 +2208,7 @@
         <v>8</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>15</v>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>61</v>
@@ -2228,18 +2228,18 @@
         <v>8</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>124</v>
@@ -2248,7 +2248,7 @@
         <v>8</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>15</v>
@@ -2259,7 +2259,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>61</v>
@@ -2268,7 +2268,7 @@
         <v>8</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>55</v>
@@ -2279,7 +2279,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>61</v>
@@ -2288,7 +2288,7 @@
         <v>8</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>55</v>
@@ -2299,7 +2299,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>61</v>
@@ -2308,7 +2308,7 @@
         <v>8</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>15</v>
@@ -2319,7 +2319,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>61</v>
@@ -2328,13 +2328,13 @@
         <v>8</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data update post-approps 9/2/25
</commit_message>
<xml_diff>
--- a/data/Bills-RUBIO-Present.xlsx
+++ b/data/Bills-RUBIO-Present.xlsx
@@ -12,14 +12,14 @@
     <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="9150"/>
   </bookViews>
   <sheets>
-    <sheet name="Bills-2025-08-25_1133" sheetId="1" r:id="rId1"/>
+    <sheet name="Bills-2025-09-02_1103" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="230">
   <si>
     <t xml:space="preserve">Measure          </t>
   </si>
@@ -57,6 +57,18 @@
     <t>Senate - Appropriations</t>
   </si>
   <si>
+    <t>AB-49</t>
+  </si>
+  <si>
+    <t>Muratsuchi</t>
+  </si>
+  <si>
+    <t>Schoolsites: immigration enforcement.</t>
+  </si>
+  <si>
+    <t>Senate - Third Reading</t>
+  </si>
+  <si>
     <t>AB-53</t>
   </si>
   <si>
@@ -81,6 +93,12 @@
     <t>Electricity and natural gas: legislation imposing mandated programs and requirements: third-party review.</t>
   </si>
   <si>
+    <t>AB-221</t>
+  </si>
+  <si>
+    <t>Tribal Nation Grant Fund.</t>
+  </si>
+  <si>
     <t>AB-260</t>
   </si>
   <si>
@@ -99,6 +117,15 @@
     <t>Fire safety: fire hazard severity zones: State Fire Marshal.</t>
   </si>
   <si>
+    <t>AB-288</t>
+  </si>
+  <si>
+    <t>McKinnor</t>
+  </si>
+  <si>
+    <t>Employment: labor organization.</t>
+  </si>
+  <si>
     <t>AB-380</t>
   </si>
   <si>
@@ -108,6 +135,12 @@
     <t>Price gouging.</t>
   </si>
   <si>
+    <t>AB-543</t>
+  </si>
+  <si>
+    <t>Medi-Cal: street medicine.</t>
+  </si>
+  <si>
     <t>AB-573</t>
   </si>
   <si>
@@ -126,9 +159,6 @@
     <t>Business: retail food.</t>
   </si>
   <si>
-    <t>Senate - Third Reading</t>
-  </si>
-  <si>
     <t>AB-594</t>
   </si>
   <si>
@@ -138,7 +168,37 @@
     <t>Student health insurance.</t>
   </si>
   <si>
-    <t xml:space="preserve">Assembly - </t>
+    <t>Enrolled</t>
+  </si>
+  <si>
+    <t>Assembly - Passed</t>
+  </si>
+  <si>
+    <t>AB-841</t>
+  </si>
+  <si>
+    <t>Patel</t>
+  </si>
+  <si>
+    <t>State Fire Marshal: personal protective equipment: battery fires.</t>
+  </si>
+  <si>
+    <t>AB-849</t>
+  </si>
+  <si>
+    <t>Soria</t>
+  </si>
+  <si>
+    <t>Health providers: medical chaperones.</t>
+  </si>
+  <si>
+    <t>AB-894</t>
+  </si>
+  <si>
+    <t>Carrillo</t>
+  </si>
+  <si>
+    <t>General acute care hospitals: patient directories.</t>
   </si>
   <si>
     <t>AB-957</t>
@@ -153,6 +213,15 @@
     <t>Senate - Business, Professions and Economic Development</t>
   </si>
   <si>
+    <t>AB-960</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Patient visitation.</t>
+  </si>
+  <si>
     <t>AB-1032</t>
   </si>
   <si>
@@ -174,6 +243,9 @@
     <t>Chaptered</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>AB-1303</t>
   </si>
   <si>
@@ -183,21 +255,18 @@
     <t>Communications: lifeline telephone service program.</t>
   </si>
   <si>
-    <t>Senate - Second Reading</t>
-  </si>
-  <si>
-    <t>AB-1468</t>
-  </si>
-  <si>
-    <t>Ethnic studies: content standards, curriculum frameworks, instructional materials, and compliance monitoring.</t>
+    <t>AB-1363</t>
+  </si>
+  <si>
+    <t>Stefani</t>
+  </si>
+  <si>
+    <t>Protective orders: Wyland’s Law.</t>
   </si>
   <si>
     <t>Introduced</t>
   </si>
   <si>
-    <t>Assembly - Education</t>
-  </si>
-  <si>
     <t>SB-15</t>
   </si>
   <si>
@@ -225,6 +294,9 @@
     <t>Threats: schools and places of worship.</t>
   </si>
   <si>
+    <t>Assembly - Third Reading</t>
+  </si>
+  <si>
     <t>SB-31</t>
   </si>
   <si>
@@ -243,9 +315,6 @@
     <t xml:space="preserve">Health care coverage: insulin. </t>
   </si>
   <si>
-    <t>Assembly - Third Reading</t>
-  </si>
-  <si>
     <t>SB-48</t>
   </si>
   <si>
@@ -264,6 +333,9 @@
     <t>Artificial intelligence models: large developers.</t>
   </si>
   <si>
+    <t>Assembly - Second Reading</t>
+  </si>
+  <si>
     <t>SB-56</t>
   </si>
   <si>
@@ -423,7 +495,7 @@
     <t>Physicians and surgeons: special faculty permits: academic medical centers.</t>
   </si>
   <si>
-    <t>Senate - Special Consent</t>
+    <t>Senate - Passed</t>
   </si>
   <si>
     <t>SB-388</t>
@@ -471,7 +543,13 @@
     <t>Workers’ compensation: death benefits.</t>
   </si>
   <si>
-    <t>Assembly - Consent</t>
+    <t>Senate - Unfinished Business</t>
+  </si>
+  <si>
+    <t>SB-473</t>
+  </si>
+  <si>
+    <t>Water corporations: demand elasticity: rates and surcharges.</t>
   </si>
   <si>
     <t>SB-491</t>
@@ -967,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1037,44 +1115,44 @@
         <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
@@ -1085,10 +1163,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
@@ -1100,7 +1178,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1120,7 +1198,7 @@
         <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1160,407 +1238,407 @@
         <v>10</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>65</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="E28" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1568,7 +1646,7 @@
         <v>102</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>8</v>
@@ -1577,124 +1655,124 @@
         <v>103</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>65</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>10</v>
@@ -1705,167 +1783,167 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="C40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>63</v>
+        <v>134</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>134</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>100</v>
+        <v>137</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>134</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>63</v>
+        <v>143</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>141</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>143</v>
@@ -1874,473 +1952,653 @@
         <v>8</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>74</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>150</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>65</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>63</v>
+        <v>167</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>65</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>174</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>63</v>
+        <v>178</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>178</v>
+        <v>86</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>65</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>63</v>
+        <v>143</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>63</v>
+        <v>186</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>184</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>186</v>
+        <v>86</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>150</v>
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>192</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>127</v>
+        <v>196</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>11</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>63</v>
+        <v>204</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>203</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>